<commit_message>
Updated DB related models
</commit_message>
<xml_diff>
--- a/Parte2/diagramas/globais/Dicionário Base de Dados.xlsx
+++ b/Parte2/diagramas/globais/Dicionário Base de Dados.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\LI4\Parte2\diagramas\globais\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\João\Desktop\Stuff\Uni\LI4\Parte2\diagramas\globais\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84186AD9-643C-4D43-AB33-C3BF5C366C7A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF363F8E-F9F6-41D8-8852-C8867BC5EBBF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{354140AB-37F7-4C16-9B07-EDA606960705}"/>
+    <workbookView xWindow="-3840" yWindow="1485" windowWidth="7935" windowHeight="9600" xr2:uid="{354140AB-37F7-4C16-9B07-EDA606960705}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="124">
   <si>
     <t>Entidade</t>
   </si>
@@ -54,9 +54,6 @@
     <t>ID</t>
   </si>
   <si>
-    <t>integer(10)</t>
-  </si>
-  <si>
     <t>Id único de cada receita</t>
   </si>
   <si>
@@ -85,9 +82,6 @@
   </si>
   <si>
     <t>Tempo esperado</t>
-  </si>
-  <si>
-    <t>time(7)</t>
   </si>
   <si>
     <t>Tempo esperado para a 
@@ -109,9 +103,6 @@
     <t>TemperaturaID</t>
   </si>
   <si>
-    <t>integer(4)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Temperatura </t>
   </si>
   <si>
@@ -158,9 +149,6 @@
     <t>Passo</t>
   </si>
   <si>
-    <t>Id único do passo</t>
-  </si>
-  <si>
     <t>Nr_Sequencia</t>
   </si>
   <si>
@@ -208,9 +196,6 @@
     <t>Imagem</t>
   </si>
   <si>
-    <t>Imagem do ingrediente</t>
-  </si>
-  <si>
     <t>Comida_Utensilio</t>
   </si>
   <si>
@@ -254,9 +239,6 @@
     <t>Dificuldade</t>
   </si>
   <si>
-    <t>integer(5)</t>
-  </si>
-  <si>
     <t>Dificuldade atribuída á receita a 
 ser avaliada</t>
   </si>
@@ -277,9 +259,6 @@
     <t>Data</t>
   </si>
   <si>
-    <t>timestamp</t>
-  </si>
-  <si>
     <t>Data da avaliação</t>
   </si>
   <si>
@@ -296,9 +275,6 @@
   </si>
   <si>
     <t>Dia da semana</t>
-  </si>
-  <si>
-    <t>integer(3)</t>
   </si>
   <si>
     <t xml:space="preserve">Dia da semana </t>
@@ -320,57 +296,12 @@
     <t>Id da receita a confecionar</t>
   </si>
   <si>
-    <t>Tentativas falhadas</t>
-  </si>
-  <si>
-    <t>Id da receita que está a ser confecionada</t>
-  </si>
-  <si>
-    <t>Id do utilizador que está a confecionar</t>
-  </si>
-  <si>
-    <t>Tentativas</t>
-  </si>
-  <si>
-    <t>Número de tentativas</t>
-  </si>
-  <si>
-    <t>confeciona_receita</t>
-  </si>
-  <si>
-    <t>AvaliacaoID</t>
-  </si>
-  <si>
-    <t>Id da avaliação efetuada</t>
-  </si>
-  <si>
-    <t>Id da receita confecionada</t>
-  </si>
-  <si>
-    <t>Tempo que demorou a confeção</t>
-  </si>
-  <si>
     <t>confeciona_passo</t>
   </si>
   <si>
-    <t>confeciona_receitaUtilizadorID</t>
-  </si>
-  <si>
-    <t>confeciona_receitaAvaliacaoID</t>
-  </si>
-  <si>
-    <t>confeciona_receitaReceitaID</t>
-  </si>
-  <si>
     <t>Id da receita</t>
   </si>
   <si>
-    <t>PassoID</t>
-  </si>
-  <si>
-    <t>Id do passo</t>
-  </si>
-  <si>
     <t>Tempo</t>
   </si>
   <si>
@@ -383,9 +314,6 @@
     <t>IngredienteID</t>
   </si>
   <si>
-    <t>Id do passo onde o ingrediente é usado</t>
-  </si>
-  <si>
     <t>Quantidade</t>
   </si>
   <si>
@@ -410,7 +338,83 @@
     <t>Pré-aquecer o forno a 200º</t>
   </si>
   <si>
-    <t>/imagem/ingrediente5</t>
+    <t>Imagem da receita após realizada</t>
+  </si>
+  <si>
+    <t>imagem/receita1</t>
+  </si>
+  <si>
+    <t>Confeção</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>bigint</t>
+  </si>
+  <si>
+    <t>varchar(512)</t>
+  </si>
+  <si>
+    <t>URL de Video</t>
+  </si>
+  <si>
+    <t>url para vídeo a demonstrar o passo</t>
+  </si>
+  <si>
+    <t>youtube.com/
+passo1</t>
+  </si>
+  <si>
+    <t>datetime</t>
+  </si>
+  <si>
+    <t>Domingo</t>
+  </si>
+  <si>
+    <t>ConfecaoID</t>
+  </si>
+  <si>
+    <t>Bem Sucedida</t>
+  </si>
+  <si>
+    <t>Usou Ajuda</t>
+  </si>
+  <si>
+    <t>PassoAtual</t>
+  </si>
+  <si>
+    <t>Id da confeção</t>
+  </si>
+  <si>
+    <t>Id do utilizador que realizou a confeção</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Id da receita </t>
+  </si>
+  <si>
+    <t>Tempo no qual foi iniciado o passo</t>
+  </si>
+  <si>
+    <t>Flag que indica se o utilizador utilizou 
+ajudas</t>
+  </si>
+  <si>
+    <t>Flag que indica se a confeção foi 
+bem sucedida</t>
+  </si>
+  <si>
+    <t>Passo da confeção em que o utilizador
+ se encontra</t>
+  </si>
+  <si>
+    <t>Início do Passo Atual</t>
+  </si>
+  <si>
+    <t>Numero do Passo</t>
+  </si>
+  <si>
+    <t>Número do passo na confeção da receita</t>
   </si>
 </sst>
 </file>
@@ -625,7 +629,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -729,6 +733,19 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1044,10 +1061,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{748C3A4C-2322-410A-A6F9-130033E694A2}">
-  <dimension ref="B2:F54"/>
+  <dimension ref="B2:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="B40" workbookViewId="0">
+      <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1059,7 +1076,7 @@
     <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1076,7 +1093,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
@@ -1084,329 +1101,330 @@
         <v>6</v>
       </c>
       <c r="D3" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="E3" s="14" t="s">
         <v>7</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>8</v>
       </c>
       <c r="F3" s="15">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="4"/>
       <c r="C4" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="E4" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="F4" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="18" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="4"/>
       <c r="C5" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="E5" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="F5" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="18" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" ht="25.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="2:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B6" s="4"/>
       <c r="C6" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="E6" s="19" t="s">
         <v>17</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="19" t="s">
-        <v>19</v>
       </c>
       <c r="F6" s="20">
         <v>1.3888888888888888E-2</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="4"/>
       <c r="C7" s="16" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>7</v>
+        <v>102</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F7" s="18">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="4"/>
       <c r="C8" s="16" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>7</v>
+        <v>102</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F8" s="18">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="4"/>
       <c r="C9" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="F9" s="18" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" s="4"/>
       <c r="C10" s="16" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>7</v>
+        <v>102</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F10" s="18">
         <v>492</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="4"/>
       <c r="C11" s="16" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>7</v>
+        <v>102</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F11" s="18">
         <v>18.2</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B12" s="4"/>
       <c r="C12" s="16" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>7</v>
+        <v>102</v>
       </c>
       <c r="E12" s="19" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F12" s="18">
         <v>42.27</v>
       </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G12" s="39"/>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="4"/>
       <c r="C13" s="16" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>7</v>
+        <v>102</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F13" s="18">
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="5"/>
-      <c r="C14" s="21" t="s">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="38"/>
+      <c r="C14" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="D14" s="22" t="s">
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="4"/>
+      <c r="C15" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" s="37" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="37" t="s">
+        <v>99</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E14" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="F14" s="23" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="F15" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B16" s="4"/>
-      <c r="C16" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="D16" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="E16" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="F16" s="18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C16" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F16" s="41" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B17" s="4"/>
       <c r="C17" s="16" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="E17" s="17" t="s">
-        <v>45</v>
+        <v>102</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>39</v>
       </c>
       <c r="F17" s="18">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" ht="25.5" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="4"/>
       <c r="C18" s="16" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>10</v>
+        <v>102</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="F18" s="24" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="F18" s="18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B19" s="4"/>
       <c r="C19" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="F19" s="24" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="4"/>
+      <c r="C20" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="E20" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="F20" s="20">
+        <v>6.9444444444444441E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B21" s="5"/>
+      <c r="C21" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="D19" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="E19" s="17" t="s">
+      <c r="F21" s="23" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F19" s="20">
-        <v>6.9444444444444441E-3</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B20" s="5"/>
-      <c r="C20" s="21" t="s">
+      <c r="C22" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="E22" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="D20" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="E20" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="F20" s="23" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E21" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="F21" s="15">
+      <c r="F22" s="15">
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="4"/>
-      <c r="C22" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D22" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="E22" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="F22" s="18" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="4"/>
       <c r="C23" s="16" t="s">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="D23" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="E23" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="F23" s="24" t="s">
-        <v>123</v>
+      <c r="F23" s="18" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="2:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B24" s="5"/>
       <c r="C24" s="21" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D24" s="22" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E24" s="25" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="F24" s="23">
         <v>1</v>
@@ -1414,16 +1432,16 @@
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C25" s="13" t="s">
         <v>6</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>7</v>
+        <v>102</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="F25" s="15">
         <v>2</v>
@@ -1432,45 +1450,45 @@
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" s="4"/>
       <c r="C26" s="16" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D26" s="17" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E26" s="17" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="F26" s="26" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" s="5"/>
       <c r="C27" s="21" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D27" s="22" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E27" s="22" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="F27" s="23" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C28" s="13" t="s">
         <v>6</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>7</v>
+        <v>102</v>
       </c>
       <c r="E28" s="14" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F28" s="15">
         <v>5</v>
@@ -1479,13 +1497,13 @@
     <row r="29" spans="2:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B29" s="4"/>
       <c r="C29" s="16" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D29" s="17" t="s">
-        <v>72</v>
+        <v>102</v>
       </c>
       <c r="E29" s="19" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F29" s="18">
         <v>5</v>
@@ -1494,13 +1512,13 @@
     <row r="30" spans="2:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B30" s="4"/>
       <c r="C30" s="16" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D30" s="17" t="s">
-        <v>72</v>
+        <v>102</v>
       </c>
       <c r="E30" s="19" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="F30" s="18">
         <v>7</v>
@@ -1509,13 +1527,13 @@
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31" s="4"/>
       <c r="C31" s="16" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D31" s="17" t="s">
-        <v>72</v>
+        <v>102</v>
       </c>
       <c r="E31" s="17" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F31" s="18">
         <v>10</v>
@@ -1524,13 +1542,13 @@
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32" s="5"/>
       <c r="C32" s="21" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="D32" s="22" t="s">
-        <v>79</v>
+        <v>108</v>
       </c>
       <c r="E32" s="22" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="F32" s="27">
         <v>43500.600694444445</v>
@@ -1538,16 +1556,16 @@
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C33" s="13" t="s">
         <v>6</v>
       </c>
       <c r="D33" s="14" t="s">
-        <v>25</v>
+        <v>102</v>
       </c>
       <c r="E33" s="14" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="F33" s="15">
         <v>1</v>
@@ -1556,45 +1574,45 @@
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" s="5"/>
       <c r="C34" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="D34" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="D34" s="22" t="s">
-        <v>10</v>
-      </c>
       <c r="E34" s="22" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="F34" s="23" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35" s="6" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C35" s="28" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="D35" s="29" t="s">
-        <v>86</v>
+        <v>34</v>
       </c>
       <c r="E35" s="29" t="s">
-        <v>87</v>
-      </c>
-      <c r="F35" s="15">
-        <v>2</v>
+        <v>79</v>
+      </c>
+      <c r="F35" s="15" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="36" spans="2:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B36" s="7"/>
       <c r="C36" s="30" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="D36" s="31" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E36" s="32" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="F36" s="18">
         <v>1</v>
@@ -1603,13 +1621,13 @@
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B37" s="7"/>
       <c r="C37" s="30" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="D37" s="31" t="s">
-        <v>7</v>
+        <v>102</v>
       </c>
       <c r="E37" s="31" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="F37" s="18">
         <v>1</v>
@@ -1618,13 +1636,13 @@
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B38" s="8"/>
       <c r="C38" s="33" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D38" s="34" t="s">
-        <v>7</v>
+        <v>102</v>
       </c>
       <c r="E38" s="34" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="F38" s="23">
         <v>1</v>
@@ -1632,93 +1650,91 @@
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B39" s="9" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="C39" s="29" t="s">
-        <v>44</v>
+        <v>110</v>
       </c>
       <c r="D39" s="29" t="s">
-        <v>7</v>
+        <v>102</v>
       </c>
       <c r="E39" s="29" t="s">
-        <v>94</v>
+        <v>114</v>
       </c>
       <c r="F39" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="10"/>
       <c r="C40" s="31" t="s">
-        <v>90</v>
+        <v>112</v>
       </c>
       <c r="D40" s="31" t="s">
-        <v>7</v>
-      </c>
-      <c r="E40" s="31" t="s">
-        <v>95</v>
+        <v>54</v>
+      </c>
+      <c r="E40" s="32" t="s">
+        <v>118</v>
       </c>
       <c r="F40" s="18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B41" s="11"/>
-      <c r="C41" s="34" t="s">
-        <v>96</v>
-      </c>
-      <c r="D41" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="E41" s="34" t="s">
-        <v>97</v>
-      </c>
-      <c r="F41" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="10"/>
+      <c r="C41" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="D41" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="E41" s="32" t="s">
+        <v>119</v>
+      </c>
+      <c r="F41" s="18">
         <v>1</v>
       </c>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B42" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="C42" s="29" t="s">
-        <v>90</v>
-      </c>
-      <c r="D42" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="E42" s="29" t="s">
-        <v>62</v>
-      </c>
-      <c r="F42" s="15">
+      <c r="B42" s="10"/>
+      <c r="C42" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="D42" s="31" t="s">
+        <v>102</v>
+      </c>
+      <c r="E42" s="31" t="s">
+        <v>115</v>
+      </c>
+      <c r="F42" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="10"/>
       <c r="C43" s="31" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="D43" s="31" t="s">
-        <v>7</v>
-      </c>
-      <c r="E43" s="31" t="s">
-        <v>100</v>
+        <v>102</v>
+      </c>
+      <c r="E43" s="32" t="s">
+        <v>120</v>
       </c>
       <c r="F43" s="18">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B44" s="10"/>
       <c r="C44" s="31" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D44" s="31" t="s">
-        <v>7</v>
+        <v>102</v>
       </c>
       <c r="E44" s="31" t="s">
-        <v>101</v>
+        <v>116</v>
       </c>
       <c r="F44" s="18">
         <v>1</v>
@@ -1727,30 +1743,30 @@
     <row r="45" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B45" s="11"/>
       <c r="C45" s="34" t="s">
-        <v>110</v>
+        <v>121</v>
       </c>
       <c r="D45" s="34" t="s">
-        <v>18</v>
+        <v>108</v>
       </c>
       <c r="E45" s="34" t="s">
-        <v>102</v>
+        <v>117</v>
       </c>
       <c r="F45" s="35">
-        <v>1.7511574074074072E-2</v>
+        <v>0.64236111111111105</v>
       </c>
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B46" s="9" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="C46" s="29" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="D46" s="29" t="s">
-        <v>7</v>
+        <v>102</v>
       </c>
       <c r="E46" s="29" t="s">
-        <v>62</v>
+        <v>114</v>
       </c>
       <c r="F46" s="15">
         <v>1</v>
@@ -1759,13 +1775,13 @@
     <row r="47" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B47" s="10"/>
       <c r="C47" s="31" t="s">
-        <v>105</v>
+        <v>40</v>
       </c>
       <c r="D47" s="31" t="s">
-        <v>7</v>
+        <v>102</v>
       </c>
       <c r="E47" s="31" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="F47" s="18">
         <v>2</v>
@@ -1774,75 +1790,75 @@
     <row r="48" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B48" s="10"/>
       <c r="C48" s="31" t="s">
-        <v>106</v>
+        <v>122</v>
       </c>
       <c r="D48" s="31" t="s">
-        <v>7</v>
+        <v>102</v>
       </c>
       <c r="E48" s="31" t="s">
-        <v>107</v>
+        <v>123</v>
       </c>
       <c r="F48" s="18">
         <v>3</v>
       </c>
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B49" s="10"/>
-      <c r="C49" s="31" t="s">
-        <v>108</v>
-      </c>
-      <c r="D49" s="31" t="s">
-        <v>7</v>
-      </c>
-      <c r="E49" s="31" t="s">
-        <v>109</v>
-      </c>
-      <c r="F49" s="18">
-        <v>4</v>
+      <c r="B49" s="11"/>
+      <c r="C49" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="D49" s="34" t="s">
+        <v>102</v>
+      </c>
+      <c r="E49" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="F49" s="35">
+        <v>3.6689814814814814E-3</v>
       </c>
     </row>
     <row r="50" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B50" s="11"/>
-      <c r="C50" s="34" t="s">
-        <v>110</v>
-      </c>
-      <c r="D50" s="34" t="s">
-        <v>18</v>
-      </c>
-      <c r="E50" s="34" t="s">
-        <v>111</v>
-      </c>
-      <c r="F50" s="35">
-        <v>3.6689814814814814E-3</v>
+      <c r="B50" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C50" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="D50" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="E50" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="F50" s="15">
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B51" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="C51" s="29" t="s">
-        <v>113</v>
-      </c>
-      <c r="D51" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="E51" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="F51" s="15">
-        <v>1</v>
+      <c r="B51" s="10"/>
+      <c r="C51" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="D51" s="40" t="s">
+        <v>102</v>
+      </c>
+      <c r="E51" s="40" t="s">
+        <v>86</v>
+      </c>
+      <c r="F51" s="18">
+        <v>2</v>
       </c>
     </row>
     <row r="52" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B52" s="10"/>
       <c r="C52" s="31" t="s">
-        <v>108</v>
+        <v>122</v>
       </c>
       <c r="D52" s="31" t="s">
-        <v>7</v>
+        <v>102</v>
       </c>
       <c r="E52" s="31" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="F52" s="18">
         <v>1</v>
@@ -1851,13 +1867,13 @@
     <row r="53" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B53" s="12"/>
       <c r="C53" s="31" t="s">
-        <v>115</v>
+        <v>91</v>
       </c>
       <c r="D53" s="31" t="s">
-        <v>7</v>
+        <v>102</v>
       </c>
       <c r="E53" s="31" t="s">
-        <v>116</v>
+        <v>92</v>
       </c>
       <c r="F53" s="18">
         <v>500</v>
@@ -1866,16 +1882,16 @@
     <row r="54" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B54" s="1"/>
       <c r="C54" s="34" t="s">
-        <v>117</v>
+        <v>93</v>
       </c>
       <c r="D54" s="36" t="s">
-        <v>118</v>
+        <v>94</v>
       </c>
       <c r="E54" s="34" t="s">
-        <v>119</v>
+        <v>95</v>
       </c>
       <c r="F54" s="23" t="s">
-        <v>120</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>